<commit_message>
Some number for cost analysis
</commit_message>
<xml_diff>
--- a/CMQA/ConOps/Cost Analysis.xlsx
+++ b/CMQA/ConOps/Cost Analysis.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Base Mission Spacecraft" sheetId="1" r:id="rId1"/>
     <sheet name="Cost Break Down" sheetId="2" r:id="rId2"/>
+    <sheet name="References" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>Insert Dummy Name Here</t>
   </si>
@@ -141,12 +142,42 @@
   </si>
   <si>
     <t>Motherboard</t>
+  </si>
+  <si>
+    <t>https://www.kjmagnetics.com/proddetail.asp?prod=D18</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>ADC folder Copper Drive</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>http://www.pumpkininc.com/content/doc/forms/pricelist.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#graduated-tape-rules/=r1v6lr</t>
+  </si>
+  <si>
+    <t>ConOps1</t>
+  </si>
+  <si>
+    <t>ConOps2 w/ Magnets</t>
+  </si>
+  <si>
+    <t>ConOps2 w/ Velcro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -759,11 +790,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,6 +994,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1685,19 +1738,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1753,14 +1810,16 @@
       <c r="C3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="70">
+        <v>5000</v>
+      </c>
       <c r="F3" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="69"/>
+      <c r="H3" s="70"/>
       <c r="J3" s="69" t="s">
         <v>35</v>
       </c>
@@ -1771,12 +1830,14 @@
       <c r="C4" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="70">
+        <v>12</v>
+      </c>
       <c r="F4" s="68"/>
       <c r="G4" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="69"/>
+      <c r="H4" s="70"/>
       <c r="J4" s="69" t="s">
         <v>36</v>
       </c>
@@ -1789,50 +1850,61 @@
       <c r="C5" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="70">
+        <v>125</v>
+      </c>
       <c r="F5" s="68"/>
       <c r="G5" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="69"/>
+      <c r="H5" s="70"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="68"/>
       <c r="C6" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="70">
+        <f>0.86*3</f>
+        <v>2.58</v>
+      </c>
       <c r="F6" s="68"/>
       <c r="G6" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="69"/>
+      <c r="H6" s="70"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="68"/>
       <c r="C7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="70">
+        <v>7980</v>
+      </c>
       <c r="F7" s="68" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="69"/>
+      <c r="H7" s="70"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="68"/>
       <c r="C8" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="70"/>
       <c r="F8" s="68"/>
       <c r="G8" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="69"/>
+      <c r="H8" s="70">
+        <v>150</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="68" t="s">
@@ -1841,24 +1913,30 @@
       <c r="C9" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="69"/>
+      <c r="D9" s="70">
+        <v>1200</v>
+      </c>
       <c r="F9" s="68"/>
       <c r="G9" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="69"/>
+      <c r="H9" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="68"/>
       <c r="C10" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="69"/>
+      <c r="D10" s="70">
+        <v>500</v>
+      </c>
       <c r="F10" s="68"/>
       <c r="G10" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="69"/>
+      <c r="H10" s="70"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="67" t="s">
@@ -1867,54 +1945,98 @@
       <c r="C11" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="70"/>
       <c r="F11" s="67" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="69"/>
+      <c r="H11" s="70"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="74" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="69"/>
+      <c r="D12" s="70">
+        <v>2250</v>
+      </c>
       <c r="F12" s="2"/>
+      <c r="G12" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="70">
+        <f>SUM(H3:H11)</f>
+        <v>150</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="68" t="s">
+        <v>3</v>
+      </c>
       <c r="C13" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="69"/>
-      <c r="F13" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D13" s="70"/>
+      <c r="F13" s="65"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="68" t="s">
-        <v>3</v>
-      </c>
+      <c r="B14" s="68"/>
       <c r="C14" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="69"/>
+        <v>13</v>
+      </c>
+      <c r="D14" s="70">
+        <v>155.88</v>
+      </c>
       <c r="F14" s="65"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
-      <c r="C15" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="69"/>
-      <c r="F15" s="65"/>
+      <c r="C15" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="70">
+        <f>SUM(D3:D14)</f>
+        <v>17225.460000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="69"/>
+      <c r="F17" s="69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="70">
+        <f>SUM(D15,H12)</f>
+        <v>17375.460000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="70">
+        <f>SUM(D15,H12,K3)</f>
+        <v>17375.460000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="70">
+        <f>SUM(D15,H12,K4)</f>
+        <v>17375.460000000003</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B12:B13"/>
+  <mergeCells count="9">
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="F1:H1"/>
@@ -1922,10 +2044,85 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" style="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More numbers, waiting on quotes for 2 things
</commit_message>
<xml_diff>
--- a/CMQA/ConOps/Cost Analysis.xlsx
+++ b/CMQA/ConOps/Cost Analysis.xlsx
@@ -176,7 +176,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -813,9 +813,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
@@ -823,163 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -987,21 +828,180 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1325,28 +1325,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="I2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="I3" s="11" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="I3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1357,9 +1357,9 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1367,14 +1367,14 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1383,13 +1383,13 @@
     </row>
     <row r="6" spans="1:20" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="55"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="38"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1397,14 +1397,14 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="38"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1412,12 +1412,12 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="55"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="55"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
+      <c r="D8" s="10"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1425,14 +1425,14 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1442,12 +1442,12 @@
     <row r="10" spans="1:20" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1455,14 +1455,14 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="38"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1471,12 +1471,12 @@
     </row>
     <row r="12" spans="1:20" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="38"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1484,14 +1484,14 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="38"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1499,12 +1499,12 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="24"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="46"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1512,15 +1512,15 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="9"/>
+      <c r="R15" s="8"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
@@ -1529,24 +1529,24 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="9"/>
+      <c r="R16" s="8"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -1558,9 +1558,9 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -1568,14 +1568,14 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="16"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="38"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -1583,145 +1583,140 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="60"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="66"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="59"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="60"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="66"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="59"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="36" t="s">
+      <c r="B22" s="65"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="59"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="60"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="66"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="41"/>
     </row>
     <row r="24" spans="1:21" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="60"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="66"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="60"/>
-      <c r="I25" s="20" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="66"/>
+      <c r="I25" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="22"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="44"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="60"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="24"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="66"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="46"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="59"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="60"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="27"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="66"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="49"/>
     </row>
     <row r="28" spans="1:21" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="59"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="60"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="66"/>
       <c r="E28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="5"/>
+      <c r="J28" s="4"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="60"/>
-      <c r="I29" s="28" t="s">
+      <c r="B29" s="65"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="66"/>
+      <c r="I29" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="30"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="52"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="59"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="60"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="32"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="66"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="54"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="59"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="60"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="32"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="66"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="54"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="59"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="60"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="32"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="66"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="54"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="63"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="35"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="69"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:K23"/>
@@ -1731,6 +1726,11 @@
     <mergeCell ref="B19:D33"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B13:D15"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1741,7 +1741,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,291 +1752,311 @@
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="F1" s="66" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="F1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="J1" s="66" t="s">
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="66"/>
-      <c r="L1" s="64"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="13" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="15">
         <v>5000</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="J3" s="69" t="s">
+      <c r="H3" s="15">
+        <v>7000</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="69"/>
+      <c r="K3" s="15">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="68"/>
-      <c r="C4" s="69" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="70">
+      <c r="D4" s="15">
         <v>12</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="69" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="70"/>
-      <c r="J4" s="69" t="s">
+      <c r="H4" s="15">
+        <v>100</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="15">
+        <v>9.7200000000000006</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="15">
         <v>125</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="69" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="72"/>
+      <c r="H5" s="15"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="70">
+      <c r="D6" s="15">
         <f>0.86*3</f>
         <v>2.58</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="69" t="s">
+      <c r="F6" s="73"/>
+      <c r="G6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="70"/>
+      <c r="H6" s="15">
+        <v>400</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
-      <c r="C7" s="69" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="15">
         <v>7980</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="G7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="70"/>
+      <c r="H7" s="15">
+        <v>5000</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
-      <c r="C8" s="69" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="69" t="s">
+      <c r="D8" s="15"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="70">
+      <c r="H8" s="15">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="15">
         <v>1200</v>
       </c>
-      <c r="F9" s="68"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="73"/>
+      <c r="G9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
-      <c r="C10" s="69" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="70">
+      <c r="D10" s="15">
         <v>500</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69" t="s">
+      <c r="F10" s="73"/>
+      <c r="G10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="70"/>
+      <c r="H10" s="15">
+        <v>400</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="F11" s="67" t="s">
+      <c r="D11" s="15">
+        <v>50</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="70"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="70">
+      <c r="D12" s="15">
         <v>2250</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="70">
+      <c r="H12" s="15">
         <f>SUM(H3:H11)</f>
-        <v>150</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="70"/>
-      <c r="F13" s="65"/>
+      <c r="D13" s="15">
+        <v>400</v>
+      </c>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
-      <c r="C14" s="69" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="70">
+      <c r="D14" s="15">
         <v>155.88</v>
       </c>
-      <c r="F14" s="65"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="70">
+      <c r="D15" s="15">
         <f>SUM(D3:D14)</f>
-        <v>17225.460000000003</v>
+        <v>17675.460000000003</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="69"/>
-      <c r="F17" s="69" t="s">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="70">
+      <c r="F18" s="15">
         <f>SUM(D15,H12)</f>
-        <v>17375.460000000003</v>
+        <v>30725.460000000003</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="70">
+      <c r="F19" s="15">
         <f>SUM(D15,H12,K3)</f>
-        <v>17375.460000000003</v>
+        <v>30750.460000000003</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="69" t="s">
+      <c r="E20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="70">
+      <c r="F20" s="15">
         <f>SUM(D15,H12,K4)</f>
-        <v>17375.460000000003</v>
+        <v>30735.180000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="F1:H1"/>
@@ -2044,8 +2064,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2063,14 +2081,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2078,7 +2096,7 @@
       <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2118,7 +2136,7 @@
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="18" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added possible antenna price
</commit_message>
<xml_diff>
--- a/CMQA/ConOps/Cost Analysis.xlsx
+++ b/CMQA/ConOps/Cost Analysis.xlsx
@@ -1741,7 +1741,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1848,7 @@
         <v>36</v>
       </c>
       <c r="K4" s="15">
-        <v>9.7200000000000006</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,9 @@
       <c r="G5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="15">
+        <v>500</v>
+      </c>
       <c r="J5" s="8"/>
       <c r="K5" s="17"/>
     </row>
@@ -1909,7 +1911,9 @@
       <c r="C8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>1000</v>
+      </c>
       <c r="F8" s="73"/>
       <c r="G8" s="14" t="s">
         <v>30</v>
@@ -1986,7 +1990,7 @@
       </c>
       <c r="H12" s="15">
         <f>SUM(H3:H11)</f>
-        <v>13050</v>
+        <v>13550</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -2017,7 +2021,7 @@
       </c>
       <c r="D15" s="15">
         <f>SUM(D3:D14)</f>
-        <v>17675.460000000003</v>
+        <v>18675.460000000003</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
@@ -2032,7 +2036,7 @@
       </c>
       <c r="F18" s="15">
         <f>SUM(D15,H12)</f>
-        <v>30725.460000000003</v>
+        <v>32225.460000000003</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
@@ -2041,7 +2045,7 @@
       </c>
       <c r="F19" s="15">
         <f>SUM(D15,H12,K3)</f>
-        <v>30750.460000000003</v>
+        <v>32250.460000000003</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
@@ -2050,7 +2054,7 @@
       </c>
       <c r="F20" s="15">
         <f>SUM(D15,H12,K4)</f>
-        <v>30735.180000000004</v>
+        <v>32325.460000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slightly updated cost, waiting on 2 quotes
</commit_message>
<xml_diff>
--- a/CMQA/ConOps/Cost Analysis.xlsx
+++ b/CMQA/ConOps/Cost Analysis.xlsx
@@ -111,9 +111,6 @@
     <t>Propellant</t>
   </si>
   <si>
-    <t>Valves</t>
-  </si>
-  <si>
     <t>Controller</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>ConOps2 w/ Velcro</t>
+  </si>
+  <si>
+    <t>Bold means waiting on quote</t>
   </si>
 </sst>
 </file>
@@ -178,8 +178,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -195,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -801,13 +809,37 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -838,6 +870,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,135 +1029,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,28 +1368,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="I2" s="32" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="I2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="I3" s="33" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="72"/>
+      <c r="I3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="35"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1357,9 +1400,9 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1367,14 +1410,14 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1387,9 +1430,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1397,14 +1440,14 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="38"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1415,9 +1458,9 @@
       <c r="B8" s="10"/>
       <c r="C8" s="1"/>
       <c r="D8" s="10"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1425,14 +1468,14 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="66"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1445,9 +1488,9 @@
       <c r="C10" s="8"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1455,14 +1498,14 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="38"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1474,9 +1517,9 @@
       <c r="C12" s="8"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="38"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1484,14 +1527,14 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="38"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1499,12 +1542,12 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="46"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="38"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="34"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1512,12 +1555,12 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="8"/>
@@ -1529,9 +1572,9 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="8"/>
@@ -1539,14 +1582,14 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="26"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -1558,9 +1601,9 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="38"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -1568,14 +1611,14 @@
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="38"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -1583,53 +1626,53 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="65"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="66"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="54"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="65"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="66"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="54"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="38"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="65"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="66"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="59"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="38"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="65"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="66"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="41"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="54"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:21" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="66"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="1"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -1639,81 +1682,81 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="65"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="66"/>
-      <c r="I25" s="42" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="54"/>
+      <c r="I25" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="65"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="66"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="46"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="54"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="34"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="65"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="66"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="54"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="37"/>
     </row>
     <row r="28" spans="1:21" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="65"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="66"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="4"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="65"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="66"/>
-      <c r="I29" s="50" t="s">
+      <c r="B29" s="53"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="54"/>
+      <c r="I29" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="51"/>
-      <c r="K29" s="52"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="65"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="66"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="54"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="54"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="42"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="65"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="66"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="54"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="54"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="42"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="65"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="66"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="54"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="54"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="42"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="67"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="57"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1741,7 +1784,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1813,7 @@
       <c r="G1" s="74"/>
       <c r="H1" s="74"/>
       <c r="J1" s="74" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" s="74"/>
       <c r="L1" s="11"/>
@@ -1797,7 +1840,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>22</v>
@@ -1823,16 +1866,16 @@
         <v>7000</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="15">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="73"/>
       <c r="C4" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="15">
         <v>12</v>
@@ -1845,7 +1888,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" s="15">
         <v>100</v>
@@ -1856,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="15">
         <v>125</v>
@@ -1866,7 +1909,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="15">
-        <v>500</v>
+        <v>130</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="17"/>
@@ -1874,7 +1917,7 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="73"/>
       <c r="C6" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="15">
         <f>0.86*3</f>
@@ -1896,7 +1939,7 @@
       <c r="D7" s="15">
         <v>7980</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="75" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="14" t="s">
@@ -1909,12 +1952,12 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="73"/>
       <c r="C8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="15">
+        <v>39</v>
+      </c>
+      <c r="D8" s="78">
         <v>1000</v>
       </c>
-      <c r="F8" s="73"/>
+      <c r="F8" s="76"/>
       <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
@@ -1927,17 +1970,17 @@
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="15">
         <v>1200</v>
       </c>
-      <c r="F9" s="73"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="14" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="15">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -1948,12 +1991,14 @@
       <c r="D10" s="15">
         <v>500</v>
       </c>
-      <c r="F10" s="73"/>
+      <c r="F10" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="15">
-        <v>400</v>
+        <v>23</v>
+      </c>
+      <c r="H10" s="78">
+        <v>8000</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -1961,18 +2006,19 @@
         <v>18</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="15">
         <v>50</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="15"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="15">
+        <f>SUM(H3:H10)</f>
+        <v>21180</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
@@ -1984,14 +2030,6 @@
       <c r="D12" s="15">
         <v>2250</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="15">
-        <f>SUM(H3:H11)</f>
-        <v>13550</v>
-      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="73" t="s">
@@ -2004,6 +2042,9 @@
         <v>400</v>
       </c>
       <c r="F13" s="12"/>
+      <c r="G13" s="79" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="73"/>
@@ -2017,7 +2058,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="15">
         <f>SUM(D3:D14)</f>
@@ -2027,47 +2068,47 @@
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="15">
-        <f>SUM(D15,H12)</f>
-        <v>32225.460000000003</v>
+        <f>SUM(D15,H11)</f>
+        <v>39855.460000000006</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="15">
-        <f>SUM(D15,H12,K3)</f>
-        <v>32250.460000000003</v>
+        <f>SUM(D15,H11,K3)</f>
+        <v>39905.460000000006</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="15">
-        <f>SUM(D15,H12,K4)</f>
-        <v>32325.460000000003</v>
+        <f>SUM(D15,H11,K4)</f>
+        <v>39955.460000000006</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2090,26 +2131,26 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -2117,15 +2158,15 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -2133,15 +2174,15 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>